<commit_message>
Push code to branch
</commit_message>
<xml_diff>
--- a/dataOfStudent.xlsx
+++ b/dataOfStudent.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1011,10 +1011,8 @@
           <t>Panha Nhean</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="B20" t="n">
+        <v>21</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1034,6 +1032,68 @@
       <c r="F20" t="inlineStr">
         <is>
           <t>image\4af95caa62234427aa6d07e128fa4e64.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Vanda Dyy</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>23</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Phnom Penh</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Class b 2025</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>image\44c795a0026549cea99c8f4d0d600342.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>dyy</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>KPC</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>B2025</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>image\0b309e35ab6d40738af04a70c6525f40.png</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Push code to chandy
</commit_message>
<xml_diff>
--- a/dataOfStudent.xlsx
+++ b/dataOfStudent.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1071,29 +1071,59 @@
           <t>dyy</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>KPC</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>B2025</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>image\0b309e35ab6d40738af04a70c6525f40.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Vanda</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>19</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>KPC</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>B2025</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>image\0b309e35ab6d40738af04a70c6525f40.png</t>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Phnom Penh</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Singer</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>image\bdef9cf1bf584c58ac5ec5e2ff915481.png</t>
         </is>
       </c>
     </row>

</xml_diff>